<commit_message>
direct commited tracked files
</commit_message>
<xml_diff>
--- a/Student_details.xlsx
+++ b/Student_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\Github\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241098D9-8F3B-4DA6-82B1-10ED0A940BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132169C1-23F9-43A1-BE0B-CD878159B412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -345,17 +348,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>